<commit_message>
Excel and Data Tables - Working with Excel files 1, Lesson 4
</commit_message>
<xml_diff>
--- a/Excel and Data Tables/FilteringCompaniesBefore2005/Data/output/CompaniesBefore2005.xlsx
+++ b/Excel and Data Tables/FilteringCompaniesBefore2005/Data/output/CompaniesBefore2005.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3289BD-E8B9-4B10-BE99-56D184302DD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F22EBA-BDAD-40F1-9636-048B0E3AB37D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>Company</t>
   </si>
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF61E05-32F8-4FBD-AAD7-E962A6DFD82B}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -391,56 +391,67 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1">
-        <v>1999</v>
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>1974</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>2003</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>1939</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>1998</v>
       </c>
     </row>

</xml_diff>